<commit_message>
Analysis in the medium distance with 2.4GHz
</commit_message>
<xml_diff>
--- a/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
+++ b/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.25643765914908</v>
+        <v>1.917154329115354</v>
       </c>
       <c r="C2" t="n">
-        <v>4.177068252326783</v>
+        <v>3.185411237504307</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4217461089859352</v>
+        <v>-0.7667619768603215</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.819492048238524</v>
+        <v>1.264053467596442</v>
       </c>
       <c r="C3" t="n">
-        <v>2.335</v>
+        <v>1.312</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7555298414867069</v>
+        <v>0.6661037641116716</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.699997667454474</v>
+        <v>1.282382578854724</v>
       </c>
       <c r="C4" t="n">
-        <v>2.14671714912281</v>
+        <v>1.344122424812032</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8136975747960313</v>
+        <v>0.6463121152129976</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.599927446011578</v>
+        <v>1.500203407079482</v>
       </c>
       <c r="C5" t="n">
-        <v>2.22250193920525</v>
+        <v>1.948729800572808</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8538407315020138</v>
+        <v>0.337554223526647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis in the far distance with 2.4GHz
</commit_message>
<xml_diff>
--- a/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
+++ b/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.917154329115354</v>
+        <v>1.934461759624336</v>
       </c>
       <c r="C2" t="n">
-        <v>3.185411237504307</v>
+        <v>3.343285591175459</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.7667619768603215</v>
+        <v>-2.437781837780359</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.264053467596442</v>
+        <v>1.167971958220894</v>
       </c>
       <c r="C3" t="n">
-        <v>1.312</v>
+        <v>1.173</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6661037641116716</v>
+        <v>0.5431565732135101</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.282382578854724</v>
+        <v>1.210393609907037</v>
       </c>
       <c r="C4" t="n">
-        <v>1.344122424812032</v>
+        <v>1.160939830827061</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6463121152129976</v>
+        <v>0.4730805793507092</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.500203407079482</v>
+        <v>1.675738519128104</v>
       </c>
       <c r="C5" t="n">
-        <v>1.948729800572808</v>
+        <v>2.600672032961413</v>
       </c>
       <c r="D5" t="n">
-        <v>0.337554223526647</v>
+        <v>-0.9358099920757432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis in the near distance with 2.4GHz
</commit_message>
<xml_diff>
--- a/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
+++ b/2-4 GHz Analysis/tables/models_metrics_in_test_set_near.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.934461759624336</v>
+        <v>2.25643765914908</v>
       </c>
       <c r="C2" t="n">
-        <v>3.343285591175459</v>
+        <v>4.177068252326783</v>
       </c>
       <c r="D2" t="n">
-        <v>-2.437781837780359</v>
+        <v>0.4217461089859352</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.167971958220894</v>
+        <v>1.819492048238524</v>
       </c>
       <c r="C3" t="n">
-        <v>1.173</v>
+        <v>2.335</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5431565732135101</v>
+        <v>0.7555298414867069</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.210393609907037</v>
+        <v>1.699997667454474</v>
       </c>
       <c r="C4" t="n">
-        <v>1.160939830827061</v>
+        <v>2.14671714912281</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4730805793507092</v>
+        <v>0.8136975747960313</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.675738519128104</v>
+        <v>1.599927446011578</v>
       </c>
       <c r="C5" t="n">
-        <v>2.600672032961413</v>
+        <v>2.22250193920525</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.9358099920757432</v>
+        <v>0.8538407315020138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>